<commit_message>
SMX readings - first commit
</commit_message>
<xml_diff>
--- a/Engage/Sogo-Performance/src/main/resources/excelfiles/Sogo_NSReadings.xlsx
+++ b/Engage/Sogo-Performance/src/main/resources/excelfiles/Sogo_NSReadings.xlsx
@@ -15,7 +15,7 @@
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="99">
   <si>
     <t>Environment</t>
   </si>
@@ -334,7 +334,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -384,8 +385,30 @@
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <u val="single"/>
+      <color indexed="12"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <u val="single"/>
+      <color indexed="12"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -396,6 +419,66 @@
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
       </patternFill>
     </fill>
     <fill>
@@ -463,7 +546,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -475,6 +558,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -765,8 +856,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="42.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="42.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -820,9 +911,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="60.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="4.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="60.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="4.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -863,10 +954,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="4.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="4.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -946,20 +1037,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="13.5703125" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="14.28515625" customWidth="1" collapsed="1"/>
-    <col min="13" max="16" width="13.7109375" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="111.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="8.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="13" max="16" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="111.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -1043,7 +1134,7 @@
       <c r="I2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="J2" s="10" t="s">
+      <c r="J2" s="17" t="s">
         <v>96</v>
       </c>
       <c r="K2" s="7" t="s">
@@ -1093,7 +1184,7 @@
       <c r="I3" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="J3" s="17" t="s">
         <v>96</v>
       </c>
       <c r="K3" s="7" t="s">
@@ -1143,7 +1234,7 @@
       <c r="I4" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="J4" s="10" t="s">
+      <c r="J4" s="17" t="s">
         <v>96</v>
       </c>
       <c r="K4" s="7" t="s">
@@ -1193,7 +1284,7 @@
       <c r="I5" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="J5" s="10" t="s">
+      <c r="J5" s="17" t="s">
         <v>96</v>
       </c>
       <c r="K5" s="7" t="s">
@@ -1243,7 +1334,7 @@
       <c r="I6" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="J6" s="10" t="s">
+      <c r="J6" s="17" t="s">
         <v>96</v>
       </c>
       <c r="K6" s="7" t="s">
@@ -1293,7 +1384,7 @@
       <c r="I7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="J7" s="10" t="s">
+      <c r="J7" s="17" t="s">
         <v>96</v>
       </c>
       <c r="K7" s="7" t="s">
@@ -1343,7 +1434,7 @@
       <c r="I8" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="J8" s="10" t="s">
+      <c r="J8" s="17" t="s">
         <v>96</v>
       </c>
       <c r="K8" s="7" t="s">
@@ -1395,7 +1486,7 @@
       <c r="I9" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="J9" s="10" t="s">
+      <c r="J9" s="17" t="s">
         <v>96</v>
       </c>
       <c r="K9" s="7" t="s">
@@ -1447,7 +1538,7 @@
       <c r="I10" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="J10" s="10" t="s">
+      <c r="J10" s="17" t="s">
         <v>96</v>
       </c>
       <c r="K10" s="7" t="s">
@@ -1499,7 +1590,7 @@
       <c r="I11" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="J11" s="10" t="s">
+      <c r="J11" s="17" t="s">
         <v>96</v>
       </c>
       <c r="K11" s="7" t="s">
@@ -1551,7 +1642,7 @@
       <c r="I12" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="J12" s="10" t="s">
+      <c r="J12" s="17" t="s">
         <v>96</v>
       </c>
       <c r="K12" s="7" t="s">
@@ -1603,7 +1694,7 @@
       <c r="I13" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="J13" s="10" t="s">
+      <c r="J13" s="17" t="s">
         <v>96</v>
       </c>
       <c r="K13" s="7" t="s">
@@ -1655,7 +1746,7 @@
       <c r="I14" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="J14" s="10" t="s">
+      <c r="J14" s="17" t="s">
         <v>96</v>
       </c>
       <c r="K14" s="7" t="s">
@@ -1707,7 +1798,7 @@
       <c r="I15" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="J15" s="10" t="s">
+      <c r="J15" s="17" t="s">
         <v>96</v>
       </c>
       <c r="K15" s="7" t="s">
@@ -1759,7 +1850,7 @@
       <c r="I16" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="J16" s="10" t="s">
+      <c r="J16" s="17" t="s">
         <v>96</v>
       </c>
       <c r="K16" s="7" t="s">
@@ -1811,7 +1902,7 @@
       <c r="I17" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="J17" s="10" t="s">
+      <c r="J17" s="17" t="s">
         <v>96</v>
       </c>
       <c r="K17" s="7" t="s">
@@ -1863,7 +1954,7 @@
       <c r="I18" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="J18" s="10" t="s">
+      <c r="J18" s="17" t="s">
         <v>96</v>
       </c>
       <c r="K18" s="7" t="s">

</xml_diff>

<commit_message>
Separated new question readings
</commit_message>
<xml_diff>
--- a/Engage/Sogo-Performance/src/main/resources/excelfiles/Sogo_NSReadings.xlsx
+++ b/Engage/Sogo-Performance/src/main/resources/excelfiles/Sogo_NSReadings.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="99">
   <si>
     <t>Environment</t>
   </si>
@@ -335,7 +335,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -407,8 +407,96 @@
       <u val="single"/>
       <color indexed="12"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <u val="single"/>
+      <color indexed="12"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <u val="single"/>
+      <color indexed="12"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <u val="single"/>
+      <color indexed="12"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <u val="single"/>
+      <color indexed="12"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <u val="single"/>
+      <color indexed="12"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <u val="single"/>
+      <color indexed="12"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <u val="single"/>
+      <color indexed="12"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <u val="single"/>
+      <color indexed="12"/>
+    </font>
   </fonts>
-  <fills count="17">
+  <fills count="65">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -419,6 +507,246 @@
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
       </patternFill>
     </fill>
     <fill>
@@ -546,7 +874,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -566,6 +894,38 @@
     <xf numFmtId="0" fontId="10" fillId="14" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
     <xf numFmtId="0" fontId="10" fillId="16" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="18" fillId="36" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="18" fillId="38" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="18" fillId="40" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="20" fillId="42" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="20" fillId="44" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="20" fillId="46" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="22" fillId="48" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="22" fillId="50" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="22" fillId="52" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="24" fillId="54" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="24" fillId="56" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="24" fillId="58" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="26" fillId="60" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="26" fillId="62" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="26" fillId="64" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1134,7 +1494,7 @@
       <c r="I2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="J2" s="17" t="s">
+      <c r="J2" s="49" t="s">
         <v>96</v>
       </c>
       <c r="K2" s="7" t="s">
@@ -1184,7 +1544,7 @@
       <c r="I3" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="17" t="s">
+      <c r="J3" s="49" t="s">
         <v>96</v>
       </c>
       <c r="K3" s="7" t="s">
@@ -1234,7 +1594,7 @@
       <c r="I4" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="J4" s="17" t="s">
+      <c r="J4" s="49" t="s">
         <v>96</v>
       </c>
       <c r="K4" s="7" t="s">
@@ -1284,7 +1644,7 @@
       <c r="I5" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="J5" s="17" t="s">
+      <c r="J5" s="49" t="s">
         <v>96</v>
       </c>
       <c r="K5" s="7" t="s">
@@ -1334,7 +1694,7 @@
       <c r="I6" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="J6" s="17" t="s">
+      <c r="J6" s="49" t="s">
         <v>96</v>
       </c>
       <c r="K6" s="7" t="s">
@@ -1384,7 +1744,7 @@
       <c r="I7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="J7" s="17" t="s">
+      <c r="J7" s="49" t="s">
         <v>96</v>
       </c>
       <c r="K7" s="7" t="s">
@@ -1434,7 +1794,7 @@
       <c r="I8" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="J8" s="17" t="s">
+      <c r="J8" s="49" t="s">
         <v>96</v>
       </c>
       <c r="K8" s="7" t="s">
@@ -1486,7 +1846,7 @@
       <c r="I9" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="J9" s="17" t="s">
+      <c r="J9" s="49" t="s">
         <v>96</v>
       </c>
       <c r="K9" s="7" t="s">
@@ -1538,7 +1898,7 @@
       <c r="I10" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="J10" s="17" t="s">
+      <c r="J10" s="49" t="s">
         <v>96</v>
       </c>
       <c r="K10" s="7" t="s">
@@ -1590,7 +1950,7 @@
       <c r="I11" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="J11" s="17" t="s">
+      <c r="J11" s="49" t="s">
         <v>96</v>
       </c>
       <c r="K11" s="7" t="s">
@@ -1642,7 +2002,7 @@
       <c r="I12" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="J12" s="17" t="s">
+      <c r="J12" s="49" t="s">
         <v>96</v>
       </c>
       <c r="K12" s="7" t="s">
@@ -1694,7 +2054,7 @@
       <c r="I13" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="J13" s="17" t="s">
+      <c r="J13" s="49" t="s">
         <v>96</v>
       </c>
       <c r="K13" s="7" t="s">
@@ -1746,7 +2106,7 @@
       <c r="I14" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="J14" s="17" t="s">
+      <c r="J14" s="49" t="s">
         <v>96</v>
       </c>
       <c r="K14" s="7" t="s">
@@ -1798,7 +2158,7 @@
       <c r="I15" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="J15" s="17" t="s">
+      <c r="J15" s="49" t="s">
         <v>96</v>
       </c>
       <c r="K15" s="7" t="s">
@@ -1850,7 +2210,7 @@
       <c r="I16" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="J16" s="17" t="s">
+      <c r="J16" s="49" t="s">
         <v>96</v>
       </c>
       <c r="K16" s="7" t="s">
@@ -1902,7 +2262,7 @@
       <c r="I17" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="J17" s="17" t="s">
+      <c r="J17" s="49" t="s">
         <v>96</v>
       </c>
       <c r="K17" s="7" t="s">
@@ -1954,7 +2314,7 @@
       <c r="I18" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="J18" s="17" t="s">
+      <c r="J18" s="49" t="s">
         <v>96</v>
       </c>
       <c r="K18" s="7" t="s">

</xml_diff>